<commit_message>
Paralllelization working for Hostinger urls in testHostingerurls with session file
</commit_message>
<xml_diff>
--- a/test-artifacts/url-reports/validated-urls.xlsx
+++ b/test-artifacts/url-reports/validated-urls.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I49"/>
+  <dimension ref="A1:I51"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -433,19 +433,19 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>TAB-4</v>
+        <v>B1-C1-T1</v>
       </c>
       <c r="B2" t="str">
-        <v>https://palegoldenrod-ant-677872.hostingersite.com/basic_page/209-description/</v>
+        <v>https://palegoldenrod-ant-677872.hostingersite.com/cas/dining-survey</v>
       </c>
       <c r="C2" t="str">
-        <v>https://palegoldenrod-ant-677872.hostingersite.com/209-description/</v>
+        <v>https://palegoldenrod-ant-677872.hostingersite.com/cas/dining-survey</v>
       </c>
       <c r="D2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E2" t="str">
-        <v>https://palegoldenrod-ant-677872.hostingersite.com/209-description/</v>
+        <v>https://palegoldenrod-ant-677872.hostingersite.com/cas/dining-survey</v>
       </c>
       <c r="F2" t="b">
         <v>1</v>
@@ -459,139 +459,175 @@
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>TAB-4</v>
+        <v>B2-C1-T3</v>
       </c>
       <c r="B3" t="str">
-        <v>https://palegoldenrod-ant-677872.hostingersite.com/basic_page/209-description/</v>
+        <v>https://palegoldenrod-ant-677872.hostingersite.com/business/fed-challenge</v>
+      </c>
+      <c r="C3" t="str">
+        <v>https://palegoldenrod-ant-677872.hostingersite.com/business/fed-challenge</v>
+      </c>
+      <c r="D3" t="b">
+        <v>0</v>
       </c>
       <c r="E3" t="str">
-        <v>https://palegoldenrod-ant-677872.hostingersite.com/basic_page/209-description/</v>
+        <v>https://palegoldenrod-ant-677872.hostingersite.com/business/fed-challenge</v>
       </c>
       <c r="F3" t="b">
         <v>1</v>
       </c>
       <c r="G3" t="str">
-        <v>failed</v>
-      </c>
-      <c r="I3" t="str">
-        <v>page.evaluate: Target page, context or browser has been closed</v>
+        <v>ok</v>
+      </c>
+      <c r="H3">
+        <v>200</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>TAB-4</v>
+        <v>B2-C1-T2</v>
       </c>
       <c r="B4" t="str">
-        <v>https://palegoldenrod-ant-677872.hostingersite.com/basic_page/342-description/</v>
+        <v>https://palegoldenrod-ant-677872.hostingersite.com/business/internship-etiquette</v>
+      </c>
+      <c r="C4" t="str">
+        <v>https://palegoldenrod-ant-677872.hostingersite.com/business/internship-etiquette</v>
+      </c>
+      <c r="D4" t="b">
+        <v>0</v>
       </c>
       <c r="E4" t="str">
-        <v>https://palegoldenrod-ant-677872.hostingersite.com/basic_page/342-description/</v>
+        <v>https://palegoldenrod-ant-677872.hostingersite.com/business/internship-etiquette</v>
       </c>
       <c r="F4" t="b">
         <v>1</v>
       </c>
       <c r="G4" t="str">
-        <v>failed</v>
-      </c>
-      <c r="I4" t="str">
-        <v>page.goto: Target page, context or browser has been closed</v>
+        <v>ok</v>
+      </c>
+      <c r="H4">
+        <v>200</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="str">
-        <v>TAB-4</v>
+        <v>B1-C2-T2</v>
       </c>
       <c r="B5" t="str">
-        <v>https://palegoldenrod-ant-677872.hostingersite.com/basic_page/fall-2014-course-offerings/</v>
+        <v>https://palegoldenrod-ant-677872.hostingersite.com/cas/download-cas-mobile-app-image</v>
+      </c>
+      <c r="C5" t="str">
+        <v>https://palegoldenrod-ant-677872.hostingersite.com/cas/download-cas-mobile-app-image</v>
+      </c>
+      <c r="D5" t="b">
+        <v>0</v>
       </c>
       <c r="E5" t="str">
-        <v>https://palegoldenrod-ant-677872.hostingersite.com/basic_page/fall-2014-course-offerings/</v>
+        <v>https://palegoldenrod-ant-677872.hostingersite.com/cas/download-cas-mobile-app-image</v>
       </c>
       <c r="F5" t="b">
         <v>1</v>
       </c>
       <c r="G5" t="str">
-        <v>failed</v>
-      </c>
-      <c r="I5" t="str">
-        <v>page.goto: Target page, context or browser has been closed</v>
+        <v>ok</v>
+      </c>
+      <c r="H5">
+        <v>200</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="str">
-        <v>TAB-4</v>
+        <v>B2-C1-T1</v>
       </c>
       <c r="B6" t="str">
-        <v>https://palegoldenrod-ant-677872.hostingersite.com/basic_page/david-dennis/</v>
+        <v>https://palegoldenrod-ant-677872.hostingersite.com/career_development/faculty-resources</v>
+      </c>
+      <c r="C6" t="str">
+        <v>https://palegoldenrod-ant-677872.hostingersite.com/career_development/faculty-resources</v>
+      </c>
+      <c r="D6" t="b">
+        <v>0</v>
       </c>
       <c r="E6" t="str">
-        <v>https://palegoldenrod-ant-677872.hostingersite.com/basic_page/david-dennis/</v>
+        <v>https://palegoldenrod-ant-677872.hostingersite.com/career_development/faculty-resources</v>
       </c>
       <c r="F6" t="b">
         <v>1</v>
       </c>
       <c r="G6" t="str">
-        <v>failed</v>
-      </c>
-      <c r="I6" t="str">
-        <v>page.goto: Target page, context or browser has been closed</v>
+        <v>ok</v>
+      </c>
+      <c r="H6">
+        <v>200</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="str">
-        <v>TAB-4</v>
+        <v>B1-C1-T2</v>
       </c>
       <c r="B7" t="str">
-        <v>https://palegoldenrod-ant-677872.hostingersite.com/basic_page/biology_club/</v>
+        <v>https://palegoldenrod-ant-677872.hostingersite.com/cas/dining-green-overview-image</v>
+      </c>
+      <c r="C7" t="str">
+        <v>https://palegoldenrod-ant-677872.hostingersite.com/cas/dining-green-overview-image</v>
+      </c>
+      <c r="D7" t="b">
+        <v>0</v>
       </c>
       <c r="E7" t="str">
-        <v>https://palegoldenrod-ant-677872.hostingersite.com/basic_page/biology_club/</v>
+        <v>https://palegoldenrod-ant-677872.hostingersite.com/cas/dining-green-overview-image</v>
       </c>
       <c r="F7" t="b">
         <v>1</v>
       </c>
       <c r="G7" t="str">
-        <v>failed</v>
-      </c>
-      <c r="I7" t="str">
-        <v>page.goto: Target page, context or browser has been closed</v>
+        <v>ok</v>
+      </c>
+      <c r="H7">
+        <v>200</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="str">
-        <v>TAB-4</v>
+        <v>B2-C1-T1</v>
       </c>
       <c r="B8" t="str">
-        <v>https://palegoldenrod-ant-677872.hostingersite.com/basic_page/facstaff_grounds/</v>
+        <v>https://palegoldenrod-ant-677872.hostingersite.com/cas/local-vendors</v>
+      </c>
+      <c r="C8" t="str">
+        <v>https://palegoldenrod-ant-677872.hostingersite.com/cas/local-vendors</v>
+      </c>
+      <c r="D8" t="b">
+        <v>0</v>
       </c>
       <c r="E8" t="str">
-        <v>https://palegoldenrod-ant-677872.hostingersite.com/basic_page/facstaff_grounds/</v>
+        <v>https://palegoldenrod-ant-677872.hostingersite.com/cas/local-vendors</v>
       </c>
       <c r="F8" t="b">
         <v>1</v>
       </c>
       <c r="G8" t="str">
-        <v>failed</v>
-      </c>
-      <c r="I8" t="str">
-        <v>page.goto: Target page, context or browser has been closed</v>
+        <v>ok</v>
+      </c>
+      <c r="H8">
+        <v>200</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="str">
-        <v>TAB-1</v>
+        <v>B1-C2-T2</v>
       </c>
       <c r="B9" t="str">
-        <v>https://palegoldenrod-ant-677872.hostingersite.com/basic_page/applied-biosystems-model-7000-real-time-thermalcycler/</v>
+        <v>https://palegoldenrod-ant-677872.hostingersite.com/cas/roomreservation</v>
       </c>
       <c r="C9" t="str">
-        <v>https://palegoldenrod-ant-677872.hostingersite.com/chemistry/applied-biosystems-model-7000-real-time-thermalcycler/</v>
+        <v>https://palegoldenrod-ant-677872.hostingersite.com/cas/roomreservation</v>
       </c>
       <c r="D9" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E9" t="str">
-        <v>https://palegoldenrod-ant-677872.hostingersite.com/chemistry/applied-biosystems-model-7000-real-time-thermalcycler/</v>
+        <v>https://palegoldenrod-ant-677872.hostingersite.com/cas/roomreservation</v>
       </c>
       <c r="F9" t="b">
         <v>1</v>
@@ -605,139 +641,175 @@
     </row>
     <row r="10">
       <c r="A10" t="str">
-        <v>TAB-1</v>
+        <v>B2-C1-T1</v>
       </c>
       <c r="B10" t="str">
-        <v>https://palegoldenrod-ant-677872.hostingersite.com/basic_page/applied-biosystems-model-7000-real-time-thermalcycler/</v>
+        <v>https://palegoldenrod-ant-677872.hostingersite.com/chang/publications</v>
+      </c>
+      <c r="C10" t="str">
+        <v>https://palegoldenrod-ant-677872.hostingersite.com/chang/publications</v>
+      </c>
+      <c r="D10" t="b">
+        <v>0</v>
       </c>
       <c r="E10" t="str">
-        <v>https://palegoldenrod-ant-677872.hostingersite.com/basic_page/applied-biosystems-model-7000-real-time-thermalcycler/</v>
+        <v>https://palegoldenrod-ant-677872.hostingersite.com/chang/publications</v>
       </c>
       <c r="F10" t="b">
         <v>1</v>
       </c>
       <c r="G10" t="str">
-        <v>failed</v>
-      </c>
-      <c r="I10" t="str">
-        <v>page.evaluate: Target page, context or browser has been closed</v>
+        <v>ok</v>
+      </c>
+      <c r="H10">
+        <v>200</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="str">
-        <v>TAB-1</v>
+        <v>B2-C2-T3</v>
       </c>
       <c r="B11" t="str">
-        <v>https://palegoldenrod-ant-677872.hostingersite.com/basic_page/301-description/</v>
+        <v>https://palegoldenrod-ant-677872.hostingersite.com/business/4-1programs</v>
+      </c>
+      <c r="C11" t="str">
+        <v>https://palegoldenrod-ant-677872.hostingersite.com/business/4-1programs</v>
+      </c>
+      <c r="D11" t="b">
+        <v>0</v>
       </c>
       <c r="E11" t="str">
-        <v>https://palegoldenrod-ant-677872.hostingersite.com/basic_page/301-description/</v>
+        <v>https://palegoldenrod-ant-677872.hostingersite.com/business/4-1programs</v>
       </c>
       <c r="F11" t="b">
         <v>1</v>
       </c>
       <c r="G11" t="str">
-        <v>failed</v>
-      </c>
-      <c r="I11" t="str">
-        <v>page.goto: Target page, context or browser has been closed</v>
+        <v>ok</v>
+      </c>
+      <c r="H11">
+        <v>200</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="str">
-        <v>TAB-1</v>
+        <v>B1-C2-T2</v>
       </c>
       <c r="B12" t="str">
-        <v>https://palegoldenrod-ant-677872.hostingersite.com/basic_page/chemical-waste-procedures/</v>
+        <v>https://palegoldenrod-ant-677872.hostingersite.com/chemistry/coy-tempcyclerii-pcr-thermalcycler</v>
+      </c>
+      <c r="C12" t="str">
+        <v>https://palegoldenrod-ant-677872.hostingersite.com/chemistry/coy-tempcyclerii-pcr-thermalcycler</v>
+      </c>
+      <c r="D12" t="b">
+        <v>0</v>
       </c>
       <c r="E12" t="str">
-        <v>https://palegoldenrod-ant-677872.hostingersite.com/basic_page/chemical-waste-procedures/</v>
+        <v>https://palegoldenrod-ant-677872.hostingersite.com/chemistry/coy-tempcyclerii-pcr-thermalcycler</v>
       </c>
       <c r="F12" t="b">
         <v>1</v>
       </c>
       <c r="G12" t="str">
-        <v>failed</v>
-      </c>
-      <c r="I12" t="str">
-        <v>page.goto: Target page, context or browser has been closed</v>
+        <v>ok</v>
+      </c>
+      <c r="H12">
+        <v>200</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="str">
-        <v>TAB-1</v>
+        <v>B1-C2-T3</v>
       </c>
       <c r="B13" t="str">
-        <v>https://palegoldenrod-ant-677872.hostingersite.com/basic_page/beakers/</v>
+        <v>https://palegoldenrod-ant-677872.hostingersite.com/cas/dining-updates-spring-2022</v>
+      </c>
+      <c r="C13" t="str">
+        <v>https://palegoldenrod-ant-677872.hostingersite.com/cas/dining-updates-spring-2022</v>
+      </c>
+      <c r="D13" t="b">
+        <v>0</v>
       </c>
       <c r="E13" t="str">
-        <v>https://palegoldenrod-ant-677872.hostingersite.com/basic_page/beakers/</v>
+        <v>https://palegoldenrod-ant-677872.hostingersite.com/cas/dining-updates-spring-2022</v>
       </c>
       <c r="F13" t="b">
         <v>1</v>
       </c>
       <c r="G13" t="str">
-        <v>failed</v>
-      </c>
-      <c r="I13" t="str">
-        <v>page.goto: Target page, context or browser has been closed</v>
+        <v>ok</v>
+      </c>
+      <c r="H13">
+        <v>200</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="str">
-        <v>TAB-1</v>
+        <v>B2-C1-T2</v>
       </c>
       <c r="B14" t="str">
-        <v>https://palegoldenrod-ant-677872.hostingersite.com/basic_page/supervisor-survey-college-work-study-process/</v>
+        <v>https://palegoldenrod-ant-677872.hostingersite.com/cas/juice-bar-photo</v>
+      </c>
+      <c r="C14" t="str">
+        <v>https://palegoldenrod-ant-677872.hostingersite.com/cas/juice-bar-photo</v>
+      </c>
+      <c r="D14" t="b">
+        <v>0</v>
       </c>
       <c r="E14" t="str">
-        <v>https://palegoldenrod-ant-677872.hostingersite.com/basic_page/supervisor-survey-college-work-study-process/</v>
+        <v>https://palegoldenrod-ant-677872.hostingersite.com/cas/juice-bar-photo</v>
       </c>
       <c r="F14" t="b">
         <v>1</v>
       </c>
       <c r="G14" t="str">
-        <v>failed</v>
-      </c>
-      <c r="I14" t="str">
-        <v>page.goto: Target page, context or browser has been closed</v>
+        <v>ok</v>
+      </c>
+      <c r="H14">
+        <v>200</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="str">
-        <v>TAB-1</v>
+        <v>B2-C1-T1</v>
       </c>
       <c r="B15" t="str">
-        <v>https://palegoldenrod-ant-677872.hostingersite.com/basic_page/facilities_services/</v>
+        <v>https://palegoldenrod-ant-677872.hostingersite.com/chemistry/hp-5890-gcms</v>
+      </c>
+      <c r="C15" t="str">
+        <v>https://palegoldenrod-ant-677872.hostingersite.com/chemistry/hp-5890-gcms</v>
+      </c>
+      <c r="D15" t="b">
+        <v>0</v>
       </c>
       <c r="E15" t="str">
-        <v>https://palegoldenrod-ant-677872.hostingersite.com/basic_page/facilities_services/</v>
+        <v>https://palegoldenrod-ant-677872.hostingersite.com/chemistry/hp-5890-gcms</v>
       </c>
       <c r="F15" t="b">
         <v>1</v>
       </c>
       <c r="G15" t="str">
-        <v>failed</v>
-      </c>
-      <c r="I15" t="str">
-        <v>page.goto: Target page, context or browser has been closed</v>
+        <v>ok</v>
+      </c>
+      <c r="H15">
+        <v>200</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="str">
-        <v>TAB-5</v>
+        <v>B1-C2-T1</v>
       </c>
       <c r="B16" t="str">
-        <v>https://palegoldenrod-ant-677872.hostingersite.com/basic_page/216-description/</v>
+        <v>https://palegoldenrod-ant-677872.hostingersite.com/cas/expresslunch</v>
       </c>
       <c r="C16" t="str">
-        <v>https://palegoldenrod-ant-677872.hostingersite.com/216-description/</v>
+        <v>https://palegoldenrod-ant-677872.hostingersite.com/cas/expresslunch</v>
       </c>
       <c r="D16" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E16" t="str">
-        <v>https://palegoldenrod-ant-677872.hostingersite.com/216-description/</v>
+        <v>https://palegoldenrod-ant-677872.hostingersite.com/cas/expresslunch</v>
       </c>
       <c r="F16" t="b">
         <v>1</v>
@@ -751,139 +823,175 @@
     </row>
     <row r="17">
       <c r="A17" t="str">
-        <v>TAB-5</v>
+        <v>B1-C2-T3</v>
       </c>
       <c r="B17" t="str">
-        <v>https://palegoldenrod-ant-677872.hostingersite.com/basic_page/216-description/</v>
+        <v>https://palegoldenrod-ant-677872.hostingersite.com/cas/ramadan-menu</v>
+      </c>
+      <c r="C17" t="str">
+        <v>https://palegoldenrod-ant-677872.hostingersite.com/cas/ramadan-menu</v>
+      </c>
+      <c r="D17" t="b">
+        <v>0</v>
       </c>
       <c r="E17" t="str">
-        <v>https://palegoldenrod-ant-677872.hostingersite.com/basic_page/216-description/</v>
+        <v>https://palegoldenrod-ant-677872.hostingersite.com/cas/ramadan-menu</v>
       </c>
       <c r="F17" t="b">
         <v>1</v>
       </c>
       <c r="G17" t="str">
-        <v>failed</v>
-      </c>
-      <c r="I17" t="str">
-        <v>page.evaluate: Target page, context or browser has been closed</v>
+        <v>ok</v>
+      </c>
+      <c r="H17">
+        <v>200</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="str">
-        <v>TAB-5</v>
+        <v>B1-C1-T2</v>
       </c>
       <c r="B18" t="str">
-        <v>https://palegoldenrod-ant-677872.hostingersite.com/basic_page/361-description/</v>
+        <v>https://palegoldenrod-ant-677872.hostingersite.com/cas/online-ordering-faq</v>
+      </c>
+      <c r="C18" t="str">
+        <v>https://palegoldenrod-ant-677872.hostingersite.com/cas/online-ordering-faq</v>
+      </c>
+      <c r="D18" t="b">
+        <v>0</v>
       </c>
       <c r="E18" t="str">
-        <v>https://palegoldenrod-ant-677872.hostingersite.com/basic_page/361-description/</v>
+        <v>https://palegoldenrod-ant-677872.hostingersite.com/cas/online-ordering-faq</v>
       </c>
       <c r="F18" t="b">
         <v>1</v>
       </c>
       <c r="G18" t="str">
-        <v>failed</v>
-      </c>
-      <c r="I18" t="str">
-        <v>page.goto: Target page, context or browser has been closed</v>
+        <v>ok</v>
+      </c>
+      <c r="H18">
+        <v>200</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="str">
-        <v>TAB-5</v>
+        <v>B2-C2-T2</v>
       </c>
       <c r="B19" t="str">
-        <v>https://palegoldenrod-ant-677872.hostingersite.com/basic_page/julian-bond/</v>
+        <v>https://palegoldenrod-ant-677872.hostingersite.com/business/accounting-related-internships</v>
+      </c>
+      <c r="C19" t="str">
+        <v>https://palegoldenrod-ant-677872.hostingersite.com/business/accounting-related-internships</v>
+      </c>
+      <c r="D19" t="b">
+        <v>0</v>
       </c>
       <c r="E19" t="str">
-        <v>https://palegoldenrod-ant-677872.hostingersite.com/basic_page/julian-bond/</v>
+        <v>https://palegoldenrod-ant-677872.hostingersite.com/business/accounting-related-internships</v>
       </c>
       <c r="F19" t="b">
         <v>1</v>
       </c>
       <c r="G19" t="str">
-        <v>failed</v>
-      </c>
-      <c r="I19" t="str">
-        <v>page.goto: Target page, context or browser has been closed</v>
+        <v>ok</v>
+      </c>
+      <c r="H19">
+        <v>200</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="str">
-        <v>TAB-5</v>
+        <v>B1-C2-T1</v>
       </c>
       <c r="B20" t="str">
-        <v>https://palegoldenrod-ant-677872.hostingersite.com/basic_page/anticipated-enrollment-questionaire/</v>
+        <v>https://palegoldenrod-ant-677872.hostingersite.com/cas/starbucks-allergen-options</v>
+      </c>
+      <c r="C20" t="str">
+        <v>https://palegoldenrod-ant-677872.hostingersite.com/cas/starbucks-allergen-options</v>
+      </c>
+      <c r="D20" t="b">
+        <v>0</v>
       </c>
       <c r="E20" t="str">
-        <v>https://palegoldenrod-ant-677872.hostingersite.com/basic_page/anticipated-enrollment-questionaire/</v>
+        <v>https://palegoldenrod-ant-677872.hostingersite.com/cas/starbucks-allergen-options</v>
       </c>
       <c r="F20" t="b">
         <v>1</v>
       </c>
       <c r="G20" t="str">
-        <v>failed</v>
-      </c>
-      <c r="I20" t="str">
-        <v>page.goto: Target page, context or browser has been closed</v>
+        <v>ok</v>
+      </c>
+      <c r="H20">
+        <v>200</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="str">
-        <v>TAB-5</v>
+        <v>B1-C1-T2</v>
       </c>
       <c r="B21" t="str">
-        <v>https://palegoldenrod-ant-677872.hostingersite.com/basic_page/roemer-arboretum-operations-assistant-position/</v>
+        <v>https://palegoldenrod-ant-677872.hostingersite.com/chemistry/chemical-waste-procedure-lis</v>
+      </c>
+      <c r="C21" t="str">
+        <v>https://palegoldenrod-ant-677872.hostingersite.com/chemistry/chemical-waste-procedure-lis</v>
+      </c>
+      <c r="D21" t="b">
+        <v>0</v>
       </c>
       <c r="E21" t="str">
-        <v>https://palegoldenrod-ant-677872.hostingersite.com/basic_page/roemer-arboretum-operations-assistant-position/</v>
+        <v>https://palegoldenrod-ant-677872.hostingersite.com/chemistry/chemical-waste-procedure-lis</v>
       </c>
       <c r="F21" t="b">
         <v>1</v>
       </c>
       <c r="G21" t="str">
-        <v>failed</v>
-      </c>
-      <c r="I21" t="str">
-        <v>page.goto: Target page, context or browser has been closed</v>
+        <v>ok</v>
+      </c>
+      <c r="H21">
+        <v>200</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="str">
-        <v>TAB-5</v>
+        <v>B1-C2-T3</v>
       </c>
       <c r="B22" t="str">
-        <v>https://palegoldenrod-ant-677872.hostingersite.com/basic_page/funnels/</v>
+        <v>https://palegoldenrod-ant-677872.hostingersite.com/chemistry/chemistry-research-project-videos</v>
+      </c>
+      <c r="C22" t="str">
+        <v>https://palegoldenrod-ant-677872.hostingersite.com/chemistry/chemistry-research-project-videos</v>
+      </c>
+      <c r="D22" t="b">
+        <v>0</v>
       </c>
       <c r="E22" t="str">
-        <v>https://palegoldenrod-ant-677872.hostingersite.com/basic_page/funnels/</v>
+        <v>https://palegoldenrod-ant-677872.hostingersite.com/chemistry/chemistry-research-project-videos</v>
       </c>
       <c r="F22" t="b">
         <v>1</v>
       </c>
       <c r="G22" t="str">
-        <v>failed</v>
-      </c>
-      <c r="I22" t="str">
-        <v>page.goto: Target page, context or browser has been closed</v>
+        <v>ok</v>
+      </c>
+      <c r="H22">
+        <v>200</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="str">
-        <v>TAB-3</v>
+        <v>B1-C2-T1</v>
       </c>
       <c r="B23" t="str">
-        <v>https://palegoldenrod-ant-677872.hostingersite.com/basic_page/119-description/</v>
+        <v>https://palegoldenrod-ant-677872.hostingersite.com/chemistry/diversity-equity-and-inclusion-geneseo-chemistry</v>
       </c>
       <c r="C23" t="str">
-        <v>https://palegoldenrod-ant-677872.hostingersite.com/119-description/</v>
+        <v>https://palegoldenrod-ant-677872.hostingersite.com/chemistry/diversity-equity-and-inclusion-geneseo-chemistry</v>
       </c>
       <c r="D23" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E23" t="str">
-        <v>https://palegoldenrod-ant-677872.hostingersite.com/119-description/</v>
+        <v>https://palegoldenrod-ant-677872.hostingersite.com/chemistry/diversity-equity-and-inclusion-geneseo-chemistry</v>
       </c>
       <c r="F23" t="b">
         <v>1</v>
@@ -897,139 +1005,175 @@
     </row>
     <row r="24">
       <c r="A24" t="str">
-        <v>TAB-3</v>
+        <v>B2-C2-T1</v>
       </c>
       <c r="B24" t="str">
-        <v>https://palegoldenrod-ant-677872.hostingersite.com/basic_page/119-description/</v>
+        <v>https://palegoldenrod-ant-677872.hostingersite.com/business/appeal-process-school-business-admission-denials</v>
+      </c>
+      <c r="C24" t="str">
+        <v>https://palegoldenrod-ant-677872.hostingersite.com/business/appeal-process-school-business-admission-denials</v>
+      </c>
+      <c r="D24" t="b">
+        <v>0</v>
       </c>
       <c r="E24" t="str">
-        <v>https://palegoldenrod-ant-677872.hostingersite.com/basic_page/119-description/</v>
+        <v>https://palegoldenrod-ant-677872.hostingersite.com/business/appeal-process-school-business-admission-denials</v>
       </c>
       <c r="F24" t="b">
         <v>1</v>
       </c>
       <c r="G24" t="str">
-        <v>failed</v>
-      </c>
-      <c r="I24" t="str">
-        <v>page.evaluate: Target page, context or browser has been closed</v>
+        <v>ok</v>
+      </c>
+      <c r="H24">
+        <v>200</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="str">
-        <v>TAB-3</v>
+        <v>B1-C2-T1</v>
       </c>
       <c r="B25" t="str">
-        <v>https://palegoldenrod-ant-677872.hostingersite.com/basic_page/331-description/</v>
+        <v>https://palegoldenrod-ant-677872.hostingersite.com/chemistry/phastsystem-electrophoresis</v>
+      </c>
+      <c r="C25" t="str">
+        <v>https://palegoldenrod-ant-677872.hostingersite.com/chemistry/phastsystem-electrophoresis</v>
+      </c>
+      <c r="D25" t="b">
+        <v>0</v>
       </c>
       <c r="E25" t="str">
-        <v>https://palegoldenrod-ant-677872.hostingersite.com/basic_page/331-description/</v>
+        <v>https://palegoldenrod-ant-677872.hostingersite.com/chemistry/phastsystem-electrophoresis</v>
       </c>
       <c r="F25" t="b">
         <v>1</v>
       </c>
       <c r="G25" t="str">
-        <v>failed</v>
-      </c>
-      <c r="I25" t="str">
-        <v>page.goto: Target page, context or browser has been closed</v>
+        <v>ok</v>
+      </c>
+      <c r="H25">
+        <v>200</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="str">
-        <v>TAB-3</v>
+        <v>B1-C1-T3</v>
       </c>
       <c r="B26" t="str">
-        <v>https://palegoldenrod-ant-677872.hostingersite.com/basic_page/past-course-offerings/</v>
+        <v>https://palegoldenrod-ant-677872.hostingersite.com/cas/board-directors-info</v>
+      </c>
+      <c r="C26" t="str">
+        <v>https://palegoldenrod-ant-677872.hostingersite.com/cas/board-directors-info</v>
+      </c>
+      <c r="D26" t="b">
+        <v>0</v>
       </c>
       <c r="E26" t="str">
-        <v>https://palegoldenrod-ant-677872.hostingersite.com/basic_page/past-course-offerings/</v>
+        <v>https://palegoldenrod-ant-677872.hostingersite.com/cas/board-directors-info</v>
       </c>
       <c r="F26" t="b">
         <v>1</v>
       </c>
       <c r="G26" t="str">
-        <v>failed</v>
-      </c>
-      <c r="I26" t="str">
-        <v>page.goto: Target page, context or browser has been closed</v>
+        <v>ok</v>
+      </c>
+      <c r="H26">
+        <v>200</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="str">
-        <v>TAB-3</v>
+        <v>B1-C1-T1</v>
       </c>
       <c r="B27" t="str">
-        <v>https://palegoldenrod-ant-677872.hostingersite.com/basic_page/charles-cobb/</v>
+        <v>https://palegoldenrod-ant-677872.hostingersite.com/cas/paintknight</v>
+      </c>
+      <c r="C27" t="str">
+        <v>https://palegoldenrod-ant-677872.hostingersite.com/cas/paintknight</v>
+      </c>
+      <c r="D27" t="b">
+        <v>0</v>
       </c>
       <c r="E27" t="str">
-        <v>https://palegoldenrod-ant-677872.hostingersite.com/basic_page/charles-cobb/</v>
+        <v>https://palegoldenrod-ant-677872.hostingersite.com/cas/paintknight</v>
       </c>
       <c r="F27" t="b">
         <v>1</v>
       </c>
       <c r="G27" t="str">
-        <v>failed</v>
-      </c>
-      <c r="I27" t="str">
-        <v>page.goto: Target page, context or browser has been closed</v>
+        <v>ok</v>
+      </c>
+      <c r="H27">
+        <v>200</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="str">
-        <v>TAB-3</v>
+        <v>B2-C2-T3</v>
       </c>
       <c r="B28" t="str">
-        <v>https://palegoldenrod-ant-677872.hostingersite.com/basic_page/exit-counseling-session-registration/</v>
+        <v>https://palegoldenrod-ant-677872.hostingersite.com/cas/feast-thrones</v>
+      </c>
+      <c r="C28" t="str">
+        <v>https://palegoldenrod-ant-677872.hostingersite.com/cas/feast-thrones</v>
+      </c>
+      <c r="D28" t="b">
+        <v>0</v>
       </c>
       <c r="E28" t="str">
-        <v>https://palegoldenrod-ant-677872.hostingersite.com/basic_page/exit-counseling-session-registration/</v>
+        <v>https://palegoldenrod-ant-677872.hostingersite.com/cas/feast-thrones</v>
       </c>
       <c r="F28" t="b">
         <v>1</v>
       </c>
       <c r="G28" t="str">
-        <v>failed</v>
-      </c>
-      <c r="I28" t="str">
-        <v>page.goto: Target page, context or browser has been closed</v>
+        <v>ok</v>
+      </c>
+      <c r="H28">
+        <v>200</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="str">
-        <v>TAB-3</v>
+        <v>B1-C1-T3</v>
       </c>
       <c r="B29" t="str">
-        <v>https://palegoldenrod-ant-677872.hostingersite.com/basic_page/chem-105-sds/</v>
+        <v>https://palegoldenrod-ant-677872.hostingersite.com/cas/ocotal-coffee</v>
+      </c>
+      <c r="C29" t="str">
+        <v>https://palegoldenrod-ant-677872.hostingersite.com/cas/ocotal-coffee</v>
+      </c>
+      <c r="D29" t="b">
+        <v>0</v>
       </c>
       <c r="E29" t="str">
-        <v>https://palegoldenrod-ant-677872.hostingersite.com/basic_page/chem-105-sds/</v>
+        <v>https://palegoldenrod-ant-677872.hostingersite.com/cas/ocotal-coffee</v>
       </c>
       <c r="F29" t="b">
         <v>1</v>
       </c>
       <c r="G29" t="str">
-        <v>failed</v>
-      </c>
-      <c r="I29" t="str">
-        <v>page.goto: Target page, context or browser has been closed</v>
+        <v>ok</v>
+      </c>
+      <c r="H29">
+        <v>200</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="str">
-        <v>TAB-2</v>
+        <v>B2-C2-T3</v>
       </c>
       <c r="B30" t="str">
-        <v>https://palegoldenrod-ant-677872.hostingersite.com/basic_page/105-description/</v>
+        <v>https://palegoldenrod-ant-677872.hostingersite.com/cas/supporting-geneseo</v>
       </c>
       <c r="C30" t="str">
-        <v>https://palegoldenrod-ant-677872.hostingersite.com/105-description/</v>
+        <v>https://palegoldenrod-ant-677872.hostingersite.com/cas/supporting-geneseo</v>
       </c>
       <c r="D30" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E30" t="str">
-        <v>https://palegoldenrod-ant-677872.hostingersite.com/105-description/</v>
+        <v>https://palegoldenrod-ant-677872.hostingersite.com/cas/supporting-geneseo</v>
       </c>
       <c r="F30" t="b">
         <v>1</v>
@@ -1043,22 +1187,22 @@
     </row>
     <row r="31">
       <c r="A31" t="str">
-        <v>TAB-2</v>
+        <v>B1-C1-T1</v>
       </c>
       <c r="B31" t="str">
-        <v>https://palegoldenrod-ant-677872.hostingersite.com/basic_page/105-description/</v>
+        <v>https://palegoldenrod-ant-677872.hostingersite.com/chemistry/chemical-waste-procedures</v>
       </c>
       <c r="C31" t="str">
-        <v>https://palegoldenrod-ant-677872.hostingersite.com/105-description/</v>
+        <v>https://palegoldenrod-ant-677872.hostingersite.com/chemistry/chemical-waste-procedures</v>
       </c>
       <c r="D31" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E31" t="str">
-        <v>https://palegoldenrod-ant-677872.hostingersite.com/wp-admin/about.php</v>
+        <v>https://palegoldenrod-ant-677872.hostingersite.com/chemistry/chemical-waste-procedures</v>
       </c>
       <c r="F31" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G31" t="str">
         <v>ok</v>
@@ -1067,50 +1211,53 @@
         <v>200</v>
       </c>
     </row>
-    <row r="32">
+    <row r="32" xml:space="preserve">
       <c r="A32" t="str">
-        <v>TAB-2</v>
+        <v>B2-C1-T3</v>
       </c>
       <c r="B32" t="str">
-        <v>https://palegoldenrod-ant-677872.hostingersite.com/basic_page/105-description/</v>
+        <v>https://palegoldenrod-ant-677872.hostingersite.com/cas/hourly-employment</v>
       </c>
       <c r="C32" t="str">
-        <v>https://palegoldenrod-ant-677872.hostingersite.com/105-description/</v>
+        <v>https://palegoldenrod-ant-677872.hostingersite.com/business/fed-challenge</v>
       </c>
       <c r="D32" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E32" t="str">
-        <v>https://palegoldenrod-ant-677872.hostingersite.com/wp-admin/contribute.php</v>
+        <v>https://palegoldenrod-ant-677872.hostingersite.com/cas/hourly-employment</v>
       </c>
       <c r="F32" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G32" t="str">
-        <v>ok</v>
-      </c>
-      <c r="H32">
-        <v>200</v>
+        <v>failed</v>
+      </c>
+      <c r="I32" t="str" xml:space="preserve">
+        <v xml:space="preserve">page.goto: Timeout 180000ms exceeded.
+Call log:
+_x001b_[2m  - navigating to "https://palegoldenrod-ant-677872.hostingersite.com/cas/hourly-employment", waiting until "domcontentloaded"_x001b_[22m
+</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="str">
-        <v>TAB-2</v>
+        <v>B2-C2-T2</v>
       </c>
       <c r="B33" t="str">
-        <v>https://palegoldenrod-ant-677872.hostingersite.com/basic_page/105-description/</v>
+        <v>https://palegoldenrod-ant-677872.hostingersite.com/cas/gf-banner</v>
       </c>
       <c r="C33" t="str">
-        <v>https://palegoldenrod-ant-677872.hostingersite.com/105-description/</v>
+        <v>https://palegoldenrod-ant-677872.hostingersite.com/cas/gf-banner</v>
       </c>
       <c r="D33" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E33" t="str">
-        <v>https://wordpress.org/</v>
+        <v>https://palegoldenrod-ant-677872.hostingersite.com/cas/gf-banner</v>
       </c>
       <c r="F33" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G33" t="str">
         <v>ok</v>
@@ -1121,22 +1268,22 @@
     </row>
     <row r="34">
       <c r="A34" t="str">
-        <v>TAB-2</v>
+        <v>B2-C1-T3</v>
       </c>
       <c r="B34" t="str">
-        <v>https://palegoldenrod-ant-677872.hostingersite.com/basic_page/105-description/</v>
+        <v>https://palegoldenrod-ant-677872.hostingersite.com/cas/winter-break-information</v>
       </c>
       <c r="C34" t="str">
-        <v>https://palegoldenrod-ant-677872.hostingersite.com/105-description/</v>
+        <v>https://palegoldenrod-ant-677872.hostingersite.com/cas/winter-break-information</v>
       </c>
       <c r="D34" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E34" t="str">
-        <v>https://wordpress.org/documentation/</v>
+        <v>https://palegoldenrod-ant-677872.hostingersite.com/cas/winter-break-information</v>
       </c>
       <c r="F34" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G34" t="str">
         <v>ok</v>
@@ -1147,22 +1294,22 @@
     </row>
     <row r="35">
       <c r="A35" t="str">
-        <v>TAB-2</v>
+        <v>B2-C2-T3</v>
       </c>
       <c r="B35" t="str">
-        <v>https://palegoldenrod-ant-677872.hostingersite.com/basic_page/105-description/</v>
+        <v>https://palegoldenrod-ant-677872.hostingersite.com/chemistry/donations-chemistry-department</v>
       </c>
       <c r="C35" t="str">
-        <v>https://palegoldenrod-ant-677872.hostingersite.com/105-description/</v>
+        <v>https://palegoldenrod-ant-677872.hostingersite.com/chemistry/donations-chemistry-department</v>
       </c>
       <c r="D35" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E35" t="str">
-        <v>https://learn.wordpress.org/</v>
+        <v>https://palegoldenrod-ant-677872.hostingersite.com/chemistry/donations-chemistry-department</v>
       </c>
       <c r="F35" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G35" t="str">
         <v>ok</v>
@@ -1173,22 +1320,22 @@
     </row>
     <row r="36">
       <c r="A36" t="str">
-        <v>TAB-2</v>
+        <v>B1-C2-T3</v>
       </c>
       <c r="B36" t="str">
-        <v>https://palegoldenrod-ant-677872.hostingersite.com/basic_page/105-description/</v>
+        <v>https://palegoldenrod-ant-677872.hostingersite.com/chemistry/nmr-software-tutorial-vnmj</v>
       </c>
       <c r="C36" t="str">
-        <v>https://palegoldenrod-ant-677872.hostingersite.com/105-description/</v>
+        <v>https://palegoldenrod-ant-677872.hostingersite.com/chemistry/nmr-software-tutorial-vnmj</v>
       </c>
       <c r="D36" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E36" t="str">
-        <v>https://wordpress.org/support/forums/</v>
+        <v>https://palegoldenrod-ant-677872.hostingersite.com/chemistry/nmr-software-tutorial-vnmj</v>
       </c>
       <c r="F36" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G36" t="str">
         <v>ok</v>
@@ -1199,22 +1346,22 @@
     </row>
     <row r="37">
       <c r="A37" t="str">
-        <v>TAB-2</v>
+        <v>B1-C1-T1</v>
       </c>
       <c r="B37" t="str">
-        <v>https://palegoldenrod-ant-677872.hostingersite.com/basic_page/105-description/</v>
+        <v>https://palegoldenrod-ant-677872.hostingersite.com/chemistry/news</v>
       </c>
       <c r="C37" t="str">
-        <v>https://palegoldenrod-ant-677872.hostingersite.com/105-description/</v>
+        <v>https://palegoldenrod-ant-677872.hostingersite.com/chemistry/news</v>
       </c>
       <c r="D37" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E37" t="str">
-        <v>https://wordpress.org/support/forum/requests-and-feedback</v>
+        <v>https://palegoldenrod-ant-677872.hostingersite.com/chemistry/news</v>
       </c>
       <c r="F37" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G37" t="str">
         <v>ok</v>
@@ -1225,22 +1372,22 @@
     </row>
     <row r="38">
       <c r="A38" t="str">
-        <v>TAB-2</v>
+        <v>B2-C1-T3</v>
       </c>
       <c r="B38" t="str">
-        <v>https://palegoldenrod-ant-677872.hostingersite.com/basic_page/105-description/</v>
+        <v>https://palegoldenrod-ant-677872.hostingersite.com/chemistry/h-cristina-geiger-publications</v>
       </c>
       <c r="C38" t="str">
-        <v>https://palegoldenrod-ant-677872.hostingersite.com/105-description/</v>
+        <v>https://palegoldenrod-ant-677872.hostingersite.com/chemistry/h-cristina-geiger-publications</v>
       </c>
       <c r="D38" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E38" t="str">
-        <v>https://palegoldenrod-ant-677872.hostingersite.com/wp-admin/</v>
+        <v>https://palegoldenrod-ant-677872.hostingersite.com/chemistry/h-cristina-geiger-publications</v>
       </c>
       <c r="F38" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G38" t="str">
         <v>ok</v>
@@ -1251,22 +1398,22 @@
     </row>
     <row r="39">
       <c r="A39" t="str">
-        <v>TAB-2</v>
+        <v>B1-C1-T2</v>
       </c>
       <c r="B39" t="str">
-        <v>https://palegoldenrod-ant-677872.hostingersite.com/basic_page/105-description/</v>
+        <v>https://palegoldenrod-ant-677872.hostingersite.com/chemistry/ndyag-laser-pumped-optical-parametric-oscillator-opo</v>
       </c>
       <c r="C39" t="str">
-        <v>https://palegoldenrod-ant-677872.hostingersite.com/105-description/</v>
+        <v>https://palegoldenrod-ant-677872.hostingersite.com/chemistry/ndyag-laser-pumped-optical-parametric-oscillator-opo</v>
       </c>
       <c r="D39" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E39" t="str">
-        <v>https://palegoldenrod-ant-677872.hostingersite.com/wp-admin/plugins.php</v>
+        <v>https://palegoldenrod-ant-677872.hostingersite.com/chemistry/ndyag-laser-pumped-optical-parametric-oscillator-opo</v>
       </c>
       <c r="F39" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G39" t="str">
         <v>ok</v>
@@ -1277,22 +1424,22 @@
     </row>
     <row r="40">
       <c r="A40" t="str">
-        <v>TAB-2</v>
+        <v>B1-C2-T2</v>
       </c>
       <c r="B40" t="str">
-        <v>https://palegoldenrod-ant-677872.hostingersite.com/basic_page/105-description/</v>
+        <v>https://palegoldenrod-ant-677872.hostingersite.com/chemistry/past_news</v>
       </c>
       <c r="C40" t="str">
-        <v>https://palegoldenrod-ant-677872.hostingersite.com/105-description/</v>
+        <v>https://palegoldenrod-ant-677872.hostingersite.com/chemistry/past_news</v>
       </c>
       <c r="D40" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E40" t="str">
-        <v>https://palegoldenrod-ant-677872.hostingersite.com/wp-admin/admin.php?page=simple_history_admin_menu_page</v>
+        <v>https://palegoldenrod-ant-677872.hostingersite.com/chemistry/past_news</v>
       </c>
       <c r="F40" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G40" t="str">
         <v>ok</v>
@@ -1303,22 +1450,22 @@
     </row>
     <row r="41">
       <c r="A41" t="str">
-        <v>TAB-2</v>
+        <v>B2-C2-T1</v>
       </c>
       <c r="B41" t="str">
-        <v>https://palegoldenrod-ant-677872.hostingersite.com/basic_page/105-description/</v>
+        <v>https://palegoldenrod-ant-677872.hostingersite.com/cas/hertz-steps</v>
       </c>
       <c r="C41" t="str">
-        <v>https://palegoldenrod-ant-677872.hostingersite.com/105-description/</v>
+        <v>https://palegoldenrod-ant-677872.hostingersite.com/cas/hertz-steps</v>
       </c>
       <c r="D41" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E41" t="str">
-        <v>https://palegoldenrod-ant-677872.hostingersite.com/wp-admin/themes.php</v>
+        <v>https://palegoldenrod-ant-677872.hostingersite.com/cas/hertz-steps</v>
       </c>
       <c r="F41" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G41" t="str">
         <v>ok</v>
@@ -1329,22 +1476,22 @@
     </row>
     <row r="42">
       <c r="A42" t="str">
-        <v>TAB-2</v>
+        <v>B2-C2-T3</v>
       </c>
       <c r="B42" t="str">
-        <v>https://palegoldenrod-ant-677872.hostingersite.com/basic_page/105-description/</v>
+        <v>https://palegoldenrod-ant-677872.hostingersite.com/chemistry/prospective_students</v>
       </c>
       <c r="C42" t="str">
-        <v>https://palegoldenrod-ant-677872.hostingersite.com/105-description/</v>
+        <v>https://palegoldenrod-ant-677872.hostingersite.com/chemistry/prospective_students</v>
       </c>
       <c r="D42" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E42" t="str">
-        <v>https://palegoldenrod-ant-677872.hostingersite.com/wp-admin/widgets.php</v>
+        <v>https://palegoldenrod-ant-677872.hostingersite.com/chemistry/prospective_students</v>
       </c>
       <c r="F42" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G42" t="str">
         <v>ok</v>
@@ -1353,182 +1500,246 @@
         <v>200</v>
       </c>
     </row>
-    <row r="43">
+    <row r="43" xml:space="preserve">
       <c r="A43" t="str">
-        <v>TAB-2</v>
+        <v>B2-C1-T2</v>
       </c>
       <c r="B43" t="str">
-        <v>https://palegoldenrod-ant-677872.hostingersite.com/basic_page/105-description/</v>
+        <v>https://palegoldenrod-ant-677872.hostingersite.com/cdl/digital-humanities</v>
       </c>
       <c r="C43" t="str">
-        <v>https://palegoldenrod-ant-677872.hostingersite.com/105-description/</v>
+        <v>https://palegoldenrod-ant-677872.hostingersite.com/cas/juice-bar-photo</v>
       </c>
       <c r="D43" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E43" t="str">
-        <v>https://palegoldenrod-ant-677872.hostingersite.com/wp-admin/nav-menus.php</v>
+        <v>https://palegoldenrod-ant-677872.hostingersite.com/cdl/digital-humanities</v>
       </c>
       <c r="F43" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G43" t="str">
-        <v>ok</v>
-      </c>
-      <c r="H43">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="44" xml:space="preserve">
+        <v>failed</v>
+      </c>
+      <c r="I43" t="str" xml:space="preserve">
+        <v xml:space="preserve">page.goto: Timeout 180000ms exceeded.
+Call log:
+_x001b_[2m  - navigating to "https://palegoldenrod-ant-677872.hostingersite.com/cdl/digital-humanities", waiting until "domcontentloaded"_x001b_[22m
+</v>
+      </c>
+    </row>
+    <row r="44">
       <c r="A44" t="str">
-        <v>TAB-2</v>
+        <v>B1-C1-T3</v>
       </c>
       <c r="B44" t="str">
-        <v>https://palegoldenrod-ant-677872.hostingersite.com/basic_page/105-description/</v>
+        <v>https://palegoldenrod-ant-677872.hostingersite.com/chemistry/brucker-avance-dpx-300-nmr-spectrometer</v>
+      </c>
+      <c r="C44" t="str">
+        <v>https://palegoldenrod-ant-677872.hostingersite.com/chemistry/brucker-avance-dpx-300-nmr-spectrometer</v>
+      </c>
+      <c r="D44" t="b">
+        <v>0</v>
       </c>
       <c r="E44" t="str">
-        <v>https://palegoldenrod-ant-677872.hostingersite.com/basic_page/105-description/</v>
+        <v>https://palegoldenrod-ant-677872.hostingersite.com/chemistry/brucker-avance-dpx-300-nmr-spectrometer</v>
       </c>
       <c r="F44" t="b">
         <v>1</v>
       </c>
       <c r="G44" t="str">
-        <v>failed</v>
-      </c>
-      <c r="I44" t="str" xml:space="preserve">
-        <v xml:space="preserve">apiRequestContext.get: Request context disposed.
-Call log:
-_x001b_[2m  - → GET https://palegoldenrod-ant-677872.hostingersite.com/wp-admin/customize.php?url=https://palegoldenrod-ant-677872.hostingersite.com/105-description/_x001b_[22m
-_x001b_[2m    - user-agent: Mozilla/5.0 (Windows NT 10.0; Win64; x64) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/140.0.7339.16 Safari/537.36_x001b_[22m
-_x001b_[2m    - accept: */*_x001b_[22m
-_x001b_[2m    - accept-encoding: gzip,deflate,br_x001b_[22m
-_x001b_[2m    - cookie: wordpress_sec_e7686b605433b6cabb072ac7f6af68b5=amit.kaushal%40infostride.com%7C1759903905%7CNMiAjexxk5gqjcBZEWZ7hzFc3kjdNmHtDjGQeDLGmlu%7C7842ea932ef361bee5a6cf362ee0a6f21ff8a8e2068dfc660e6d926ddc1d03d2; hcdn=AQEA7Z50zo1WmNFjoUBrt1un8k4R3Eth4W7CgdjrzQI9jHqfXeNoAAAAAAAQAQDhx6UaRFWAJLIbX9dMwStuAAAA3mvFcxRMqv3jZ7XVOPNJYQ; PHPSESSID=tmuk6fkj8elg4s1g1q8bafsvt2; wordpress_test_cookie=WP%20Cookie%20check; wordpress_logged_in_e7686b605433b6cabb072ac7f6af68b5=amit.kaushal%40infostride.com%7C1759903905%7CNMiAjexxk5gqjcBZEWZ7hzFc3kjdNmHtDjGQeDLGmlu%7C4fe16b92984be246d057e1c9995ae4c62f1f08130d858b433ee35f5aee042c2a; wp-settings-2=libraryContent%3Dbrowse%26posts_list_mode%3Dlist; wp-settings-time-2=1759731106_x001b_[22m
-_x001b_[2m  - ← 200 OK_x001b_[22m
-_x001b_[2m    - date: Mon, 06 Oct 2025 06:13:03 GMT_x001b_[22m
-_x001b_[2m    - content-type: text/html; charset=UTF-8_x001b_[22m
-_x001b_[2m    - transfer-encoding: chunked_x001b_[22m
-_x001b_[2m    - connection: keep-alive_x001b_[22m
-_x001b_[2m    - vary: Accept-Encoding_x001b_[22m
-_x001b_[2m    - x-powered-by: PHP/8.2.27_x001b_[22m
-_x001b_[2m    - pragma: no-cache_x001b_[22m
-_x001b_[2m    - expires: Wed, 11 Jan 1984 05:00:00 GMT_x001b_[22m
-_x001b_[2m    - cache-control: no-cache, must-revalidate, max-age=0, no-store, private_x001b_[22m
-_x001b_[2m    - referrer-policy: strict-origin-when-cross-origin_x001b_[22m
-_x001b_[2m    - x-frame-options: SAMEORIGIN_x001b_[22m
-_x001b_[2m    - platform: hostinger_x001b_[22m
-_x001b_[2m    - panel: hpanel_x001b_[22m
-_x001b_[2m    - content-security-policy: upgrade-insecure-requests_x001b_[22m
-_x001b_[2m    - server: hcdn_x001b_[22m
-_x001b_[2m    - x-hcdn-request-id: 76696b6915336713db482f736bf6ebfe-mum-edge9_x001b_[22m
-_x001b_[2m    - x-hcdn-cache-status: DYNAMIC_x001b_[22m
-_x001b_[2m    - x-hcdn-upstream-rt: 1.765_x001b_[22m
-_x001b_[2m    - content-encoding: br_x001b_[22m
-</v>
+        <v>ok</v>
+      </c>
+      <c r="H44">
+        <v>200</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="str">
-        <v>TAB-2</v>
+        <v>B2-C2-T2</v>
       </c>
       <c r="B45" t="str">
-        <v>https://palegoldenrod-ant-677872.hostingersite.com/basic_page/313-description/</v>
+        <v>https://palegoldenrod-ant-677872.hostingersite.com/cas/VeganDinner</v>
+      </c>
+      <c r="C45" t="str">
+        <v>https://palegoldenrod-ant-677872.hostingersite.com/cas/VeganDinner</v>
+      </c>
+      <c r="D45" t="b">
+        <v>0</v>
       </c>
       <c r="E45" t="str">
-        <v>https://palegoldenrod-ant-677872.hostingersite.com/basic_page/313-description/</v>
+        <v>https://palegoldenrod-ant-677872.hostingersite.com/cas/VeganDinner</v>
       </c>
       <c r="F45" t="b">
         <v>1</v>
       </c>
       <c r="G45" t="str">
-        <v>failed</v>
-      </c>
-      <c r="I45" t="str">
-        <v>page.goto: Target page, context or browser has been closed</v>
+        <v>ok</v>
+      </c>
+      <c r="H45">
+        <v>200</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="str">
-        <v>TAB-2</v>
+        <v>B2-C2-T1</v>
       </c>
       <c r="B46" t="str">
-        <v>https://palegoldenrod-ant-677872.hostingersite.com/basic_page/construction-page-chemical-safety/</v>
+        <v>https://palegoldenrod-ant-677872.hostingersite.com/cas/webform/fast-account-contact-form</v>
+      </c>
+      <c r="C46" t="str">
+        <v>https://palegoldenrod-ant-677872.hostingersite.com/cas/webform/fast-account-contact-form</v>
+      </c>
+      <c r="D46" t="b">
+        <v>0</v>
       </c>
       <c r="E46" t="str">
-        <v>https://palegoldenrod-ant-677872.hostingersite.com/basic_page/construction-page-chemical-safety/</v>
+        <v>https://palegoldenrod-ant-677872.hostingersite.com/cas/webform/fast-account-contact-form</v>
       </c>
       <c r="F46" t="b">
         <v>1</v>
       </c>
       <c r="G46" t="str">
-        <v>failed</v>
-      </c>
-      <c r="I46" t="str">
-        <v>page.goto: Target page, context or browser has been closed</v>
+        <v>ok</v>
+      </c>
+      <c r="H46">
+        <v>200</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="str">
-        <v>TAB-2</v>
+        <v>B1-C1-T3</v>
       </c>
       <c r="B47" t="str">
-        <v>https://palegoldenrod-ant-677872.hostingersite.com/basic_page/peace_action/</v>
+        <v>https://palegoldenrod-ant-677872.hostingersite.com/chemistry/marathon-16-km-ultracentrafuge</v>
+      </c>
+      <c r="C47" t="str">
+        <v>https://palegoldenrod-ant-677872.hostingersite.com/chemistry/marathon-16-km-ultracentrafuge</v>
+      </c>
+      <c r="D47" t="b">
+        <v>0</v>
       </c>
       <c r="E47" t="str">
-        <v>https://palegoldenrod-ant-677872.hostingersite.com/basic_page/peace_action/</v>
+        <v>https://palegoldenrod-ant-677872.hostingersite.com/chemistry/marathon-16-km-ultracentrafuge</v>
       </c>
       <c r="F47" t="b">
         <v>1</v>
       </c>
       <c r="G47" t="str">
-        <v>failed</v>
-      </c>
-      <c r="I47" t="str">
-        <v>page.goto: Target page, context or browser has been closed</v>
+        <v>ok</v>
+      </c>
+      <c r="H47">
+        <v>200</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="str">
-        <v>TAB-2</v>
+        <v>B2-C2-T2</v>
       </c>
       <c r="B48" t="str">
-        <v>https://palegoldenrod-ant-677872.hostingersite.com/basic_page/hasan-jeffries/</v>
+        <v>https://palegoldenrod-ant-677872.hostingersite.com/chemistry/facstaff_chem</v>
+      </c>
+      <c r="C48" t="str">
+        <v>https://palegoldenrod-ant-677872.hostingersite.com/chemistry/facstaff_chem</v>
+      </c>
+      <c r="D48" t="b">
+        <v>0</v>
       </c>
       <c r="E48" t="str">
-        <v>https://palegoldenrod-ant-677872.hostingersite.com/basic_page/hasan-jeffries/</v>
+        <v>https://palegoldenrod-ant-677872.hostingersite.com/chemistry/facstaff_chem</v>
       </c>
       <c r="F48" t="b">
         <v>1</v>
       </c>
       <c r="G48" t="str">
-        <v>failed</v>
-      </c>
-      <c r="I48" t="str">
-        <v>page.goto: Target page, context or browser has been closed</v>
+        <v>ok</v>
+      </c>
+      <c r="H48">
+        <v>200</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="str">
-        <v>TAB-2</v>
+        <v>B2-C1-T2</v>
       </c>
       <c r="B49" t="str">
-        <v>https://palegoldenrod-ant-677872.hostingersite.com/basic_page/charles-mcdew/</v>
+        <v>https://palegoldenrod-ant-677872.hostingersite.com/chemistry/hazardous-waste-training</v>
+      </c>
+      <c r="C49" t="str">
+        <v>https://palegoldenrod-ant-677872.hostingersite.com/chemistry/hazardous-waste-training</v>
+      </c>
+      <c r="D49" t="b">
+        <v>0</v>
       </c>
       <c r="E49" t="str">
-        <v>https://palegoldenrod-ant-677872.hostingersite.com/basic_page/charles-mcdew/</v>
+        <v>https://palegoldenrod-ant-677872.hostingersite.com/chemistry/hazardous-waste-training</v>
       </c>
       <c r="F49" t="b">
         <v>1</v>
       </c>
       <c r="G49" t="str">
-        <v>failed</v>
-      </c>
-      <c r="I49" t="str">
-        <v>page.goto: Target page, context or browser has been closed</v>
+        <v>ok</v>
+      </c>
+      <c r="H49">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="str">
+        <v>B2-C2-T2</v>
+      </c>
+      <c r="B50" t="str">
+        <v>https://palegoldenrod-ant-677872.hostingersite.com/chemistry/research_oxford</v>
+      </c>
+      <c r="C50" t="str">
+        <v>https://palegoldenrod-ant-677872.hostingersite.com/chemistry/research_oxford</v>
+      </c>
+      <c r="D50" t="b">
+        <v>0</v>
+      </c>
+      <c r="E50" t="str">
+        <v>https://palegoldenrod-ant-677872.hostingersite.com/chemistry/research_oxford</v>
+      </c>
+      <c r="F50" t="b">
+        <v>1</v>
+      </c>
+      <c r="G50" t="str">
+        <v>ok</v>
+      </c>
+      <c r="H50">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="str">
+        <v>B2-C2-T1</v>
+      </c>
+      <c r="B51" t="str">
+        <v>https://palegoldenrod-ant-677872.hostingersite.com/chemistry/gamma_sigma_epsilon</v>
+      </c>
+      <c r="C51" t="str">
+        <v>https://palegoldenrod-ant-677872.hostingersite.com/chemistry/gamma_sigma_epsilon</v>
+      </c>
+      <c r="D51" t="b">
+        <v>0</v>
+      </c>
+      <c r="E51" t="str">
+        <v>https://palegoldenrod-ant-677872.hostingersite.com/chemistry/gamma_sigma_epsilon</v>
+      </c>
+      <c r="F51" t="b">
+        <v>1</v>
+      </c>
+      <c r="G51" t="str">
+        <v>ok</v>
+      </c>
+      <c r="H51">
+        <v>200</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:I49"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:I51"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>